<commit_message>
update rumus analisis dan prepos
</commit_message>
<xml_diff>
--- a/data/dataset_sekunder_2.xlsx
+++ b/data/dataset_sekunder_2.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5010c15d569d2076/04. University of Jember/01. Physics Academics/TUGAS AKHIR/04. Program-Evapotranspiration-Analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3C07439-D576-4D1A-89AC-4DB3CDDCF239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{5FC4AE24-6BC0-43CE-840C-D18D6B36F4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA7F9046-FDE2-4A2D-BBE2-990726A85A60}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="866" activeTab="4" xr2:uid="{8E10AA64-040F-43D2-8A09-EDDE4C03F492}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="866" activeTab="9" xr2:uid="{8E10AA64-040F-43D2-8A09-EDDE4C03F492}"/>
   </bookViews>
   <sheets>
-    <sheet name="day 05" sheetId="6" r:id="rId1"/>
+    <sheet name="day 05" sheetId="25" r:id="rId1"/>
     <sheet name="day 06" sheetId="7" r:id="rId2"/>
     <sheet name="day 07" sheetId="8" r:id="rId3"/>
     <sheet name="day 08" sheetId="9" r:id="rId4"/>
@@ -23,15 +23,13 @@
     <sheet name="day 13" sheetId="18" r:id="rId8"/>
     <sheet name="day 14" sheetId="19" r:id="rId9"/>
     <sheet name="day 15" sheetId="20" r:id="rId10"/>
-    <sheet name="day 16" sheetId="21" r:id="rId11"/>
-    <sheet name="day 19" sheetId="24" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="7">
   <si>
     <t>DY</t>
   </si>
@@ -911,11 +909,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E60D2C9-C4D1-4F86-9801-56869DCA6807}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D5D5BE-5732-409F-9DAC-5E8D2887F27A}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1136,7 +1134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E647E41-F596-48DA-BF34-1C023E7BEDCC}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -1347,450 +1345,6 @@
       </c>
       <c r="G9">
         <v>3.47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD366F17-AD27-415E-9846-BD449F958BAC}">
-  <dimension ref="A1:G9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>26.8</v>
-      </c>
-      <c r="D2">
-        <v>15.62</v>
-      </c>
-      <c r="E2">
-        <v>67.12</v>
-      </c>
-      <c r="F2">
-        <v>0.01</v>
-      </c>
-      <c r="G2">
-        <v>3.33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>29.31</v>
-      </c>
-      <c r="D3">
-        <v>13.98</v>
-      </c>
-      <c r="E3">
-        <v>51.94</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>3.43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>31.23</v>
-      </c>
-      <c r="D4">
-        <v>12.88</v>
-      </c>
-      <c r="E4">
-        <v>42.81</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>3.51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>32.78</v>
-      </c>
-      <c r="D5">
-        <v>12.08</v>
-      </c>
-      <c r="E5">
-        <v>36.880000000000003</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>3.58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>33.85</v>
-      </c>
-      <c r="D6">
-        <v>11.6</v>
-      </c>
-      <c r="E6">
-        <v>33.25</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>3.63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>34.380000000000003</v>
-      </c>
-      <c r="D7">
-        <v>11.47</v>
-      </c>
-      <c r="E7">
-        <v>31.88</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>3.57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <v>34.4</v>
-      </c>
-      <c r="D8">
-        <v>11.54</v>
-      </c>
-      <c r="E8">
-        <v>32</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>3.44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>15</v>
-      </c>
-      <c r="C9">
-        <v>33.979999999999997</v>
-      </c>
-      <c r="D9">
-        <v>11.66</v>
-      </c>
-      <c r="E9">
-        <v>33.19</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>3.24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10124110-D873-4F13-A9DF-B4E0FEB08258}">
-  <dimension ref="A1:G9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>26.33</v>
-      </c>
-      <c r="D2">
-        <v>17.82</v>
-      </c>
-      <c r="E2">
-        <v>78.38</v>
-      </c>
-      <c r="F2">
-        <v>0.21</v>
-      </c>
-      <c r="G2">
-        <v>2.5299999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>27.72</v>
-      </c>
-      <c r="D3">
-        <v>17.09</v>
-      </c>
-      <c r="E3">
-        <v>69.38</v>
-      </c>
-      <c r="F3">
-        <v>0.21</v>
-      </c>
-      <c r="G3">
-        <v>2.44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>28.87</v>
-      </c>
-      <c r="D4">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="E4">
-        <v>63</v>
-      </c>
-      <c r="F4">
-        <v>0.15</v>
-      </c>
-      <c r="G4">
-        <v>2.44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>29.84</v>
-      </c>
-      <c r="D5">
-        <v>16.36</v>
-      </c>
-      <c r="E5">
-        <v>58.69</v>
-      </c>
-      <c r="F5">
-        <v>0.16</v>
-      </c>
-      <c r="G5">
-        <v>2.5299999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>30.43</v>
-      </c>
-      <c r="D6">
-        <v>16.239999999999998</v>
-      </c>
-      <c r="E6">
-        <v>56.25</v>
-      </c>
-      <c r="F6">
-        <v>0.18</v>
-      </c>
-      <c r="G6">
-        <v>2.46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>30.64</v>
-      </c>
-      <c r="D7">
-        <v>16.170000000000002</v>
-      </c>
-      <c r="E7">
-        <v>55.31</v>
-      </c>
-      <c r="F7">
-        <v>0.23</v>
-      </c>
-      <c r="G7">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <v>30.55</v>
-      </c>
-      <c r="D8">
-        <v>16.170000000000002</v>
-      </c>
-      <c r="E8">
-        <v>55.62</v>
-      </c>
-      <c r="F8">
-        <v>0.36</v>
-      </c>
-      <c r="G8">
-        <v>2.15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>15</v>
-      </c>
-      <c r="C9">
-        <v>29.91</v>
-      </c>
-      <c r="D9">
-        <v>16.11</v>
-      </c>
-      <c r="E9">
-        <v>57.56</v>
-      </c>
-      <c r="F9">
-        <v>0.38</v>
-      </c>
-      <c r="G9">
-        <v>1.95</v>
       </c>
     </row>
   </sheetData>
@@ -2468,7 +2022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{014CB23E-8F07-4E5D-9BA5-7336F2EB5F36}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>

</xml_diff>